<commit_message>
- added analysis of ILRI probiotic trial data - completed intervention simulation for antimicrobial replacement intervention
</commit_message>
<xml_diff>
--- a/Intervention 1/Scenario Analysis All.xlsx
+++ b/Intervention 1/Scenario Analysis All.xlsx
@@ -94,10 +94,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1.855036680458912E9</v>
+        <v>-4.383343486795609E9</v>
       </c>
       <c r="C2" t="n">
-        <v>1.8034494257762246E9</v>
+        <v>-4.385389245879074E9</v>
       </c>
     </row>
     <row r="3">
@@ -105,10 +105,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.8519874106234527E9</v>
+        <v>-4.379616096379884E9</v>
       </c>
       <c r="C3" t="n">
-        <v>1.802070961130211E9</v>
+        <v>-4.383707625275123E9</v>
       </c>
     </row>
     <row r="4">
@@ -116,10 +116,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.7765665060470078E9</v>
+        <v>-4.37216126397213E9</v>
       </c>
       <c r="C4" t="n">
-        <v>1.7765665060470078E9</v>
+        <v>-4.380344364676104E9</v>
       </c>
     </row>
     <row r="5">
@@ -127,10 +127,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.838570691090475E9</v>
+        <v>-4.363215374307608E9</v>
       </c>
       <c r="C5" t="n">
-        <v>1.7960057435524395E9</v>
+        <v>-4.376308417828602E9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>